<commit_message>
listados listos para el 27 de julio 2024
</commit_message>
<xml_diff>
--- a/Julio/27 julio/cerro azul/PLANTILLA LISTA DE ASPIRANTES_IT_CERRO_AZUL.xlsx
+++ b/Julio/27 julio/cerro azul/PLANTILLA LISTA DE ASPIRANTES_IT_CERRO_AZUL.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Proyecto01TICs\Documents\Evaluatec2024\Julio\27 julio\cerro azul\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D6B0DDA-DE61-4789-9678-56AA5E8C361D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{946FCA35-5A75-450E-AF6D-2BDC6C5A6BBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3255" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EVALUATEC" sheetId="1" r:id="rId1"/>
@@ -2773,25 +2773,25 @@
   </sheetPr>
   <dimension ref="A1:O697"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A180" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
-      <selection activeCell="A180" sqref="A180:A285"/>
+    <sheetView tabSelected="1" topLeftCell="A322" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A362"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.375" customWidth="1"/>
-    <col min="2" max="2" width="40" style="2" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="7.375" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="47.75" style="2" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="16" style="1" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="40" style="2" customWidth="1"/>
+    <col min="3" max="3" width="7.375" customWidth="1"/>
+    <col min="4" max="4" width="47.75" style="2" customWidth="1"/>
+    <col min="5" max="5" width="16" style="1" customWidth="1"/>
     <col min="6" max="6" width="32.875" customWidth="1"/>
-    <col min="7" max="7" width="13.5" style="1" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="14.5" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="16.75" style="9" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5" style="1" customWidth="1"/>
+    <col min="8" max="8" width="14.5" customWidth="1"/>
+    <col min="9" max="9" width="16.75" style="9" customWidth="1"/>
     <col min="10" max="10" width="22.375" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="21.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="25" style="9" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="11.125" style="2" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="25" style="9" customWidth="1"/>
+    <col min="13" max="13" width="11.125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">

</xml_diff>